<commit_message>
feito as tabelas e crud-generico, DER, modelo logico e dicionario
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Tarefa</t>
   </si>
@@ -81,9 +81,6 @@
     <t>logica completa do cadastro de reservas</t>
   </si>
   <si>
-    <t>Relatorio no documento de requisitos dos DLL e MDL</t>
-  </si>
-  <si>
     <t>OBS</t>
   </si>
   <si>
@@ -93,9 +90,6 @@
     <t xml:space="preserve">Implemetação do madança de senha </t>
   </si>
   <si>
-    <t>Está incluso: a criação de todas as classe, bem como a organização delas</t>
-  </si>
-  <si>
     <t>Atualização na documentação</t>
   </si>
   <si>
@@ -148,6 +142,15 @@
   </si>
   <si>
     <t xml:space="preserve">Completude do projeto </t>
+  </si>
+  <si>
+    <t>Relatorio no documento de requisitos dos DLL</t>
+  </si>
+  <si>
+    <t>Relatorio no documento de requisitos dos MDL</t>
+  </si>
+  <si>
+    <t>Está incluso: a criação de todas as classes, bem como a organização delas.</t>
   </si>
 </sst>
 </file>
@@ -191,10 +194,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,7 +504,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,7 +537,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -592,7 +597,7 @@
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -611,8 +616,8 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -634,39 +639,39 @@
       <c r="F6" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
-        <v>25</v>
+      <c r="G6" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B7" s="1">
-        <v>43418</v>
+        <v>43416</v>
       </c>
       <c r="C7" s="1">
-        <v>43420</v>
+        <v>43417</v>
       </c>
       <c r="D7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
-        <v>43421</v>
+        <v>43418</v>
       </c>
       <c r="C8" s="1">
-        <v>43423</v>
+        <v>43420</v>
       </c>
       <c r="D8">
         <v>2</v>
@@ -680,13 +685,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1">
-        <v>43424</v>
+        <v>43421</v>
       </c>
       <c r="C9" s="1">
-        <v>43426</v>
+        <v>43423</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -700,16 +705,16 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
-        <v>43427</v>
+        <v>43424</v>
       </c>
       <c r="C10" s="1">
-        <v>43430</v>
+        <v>43426</v>
       </c>
       <c r="D10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E10" t="s">
         <v>18</v>
@@ -720,56 +725,56 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
-        <v>43431</v>
+        <v>43427</v>
       </c>
       <c r="C11" s="1">
-        <v>43431</v>
+        <v>43430</v>
       </c>
       <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="4">
+        <v>43429</v>
+      </c>
+      <c r="C12" s="4">
+        <v>43430</v>
+      </c>
+      <c r="D12" s="3">
         <v>1</v>
       </c>
-      <c r="E11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" s="1">
-        <v>43431</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43437</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
-      </c>
-      <c r="E12" t="s">
-        <v>11</v>
-      </c>
-      <c r="F12" t="s">
+      <c r="E12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
-        <v>43438</v>
+        <v>43431</v>
       </c>
       <c r="C13" s="1">
-        <v>43440</v>
+        <v>43437</v>
       </c>
       <c r="D13">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -778,24 +783,24 @@
         <v>14</v>
       </c>
       <c r="G13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1">
-        <v>43441</v>
+        <v>43438</v>
       </c>
       <c r="C14" s="1">
-        <v>43444</v>
+        <v>43440</v>
       </c>
       <c r="D14">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E14" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -803,16 +808,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B15" s="1">
         <v>43441</v>
       </c>
       <c r="C15" s="1">
-        <v>43449</v>
+        <v>43444</v>
       </c>
       <c r="D15">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
@@ -823,7 +828,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B16" s="1">
         <v>43441</v>
@@ -843,7 +848,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B17" s="1">
         <v>43441</v>
@@ -863,7 +868,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B18" s="1">
         <v>43441</v>
@@ -883,7 +888,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B19" s="1">
         <v>43441</v>
@@ -903,7 +908,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B20" s="1">
         <v>43441</v>
@@ -923,7 +928,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B21" s="1">
         <v>43441</v>
@@ -943,13 +948,13 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1">
-        <v>43450</v>
+        <v>43441</v>
       </c>
       <c r="C22" s="1">
-        <v>43457</v>
+        <v>43449</v>
       </c>
       <c r="D22">
         <v>8</v>
@@ -963,7 +968,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>43450</v>
@@ -983,7 +988,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>43450</v>
@@ -1003,7 +1008,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B25" s="1">
         <v>43450</v>
@@ -1023,7 +1028,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B26" s="1">
         <v>43450</v>
@@ -1043,7 +1048,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B27" s="1">
         <v>43450</v>
@@ -1063,16 +1068,16 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
-        <v>43458</v>
+        <v>43450</v>
       </c>
       <c r="C28" s="1">
-        <v>43479</v>
+        <v>43457</v>
       </c>
       <c r="D28">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="E28" t="s">
         <v>18</v>
@@ -1083,27 +1088,43 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B29" s="1">
+        <v>43458</v>
+      </c>
+      <c r="C29" s="1">
         <v>43479</v>
       </c>
-      <c r="C29" s="1">
+      <c r="D29">
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="1">
+        <v>43479</v>
+      </c>
+      <c r="C30" s="1">
         <v>43490</v>
       </c>
-      <c r="D29">
+      <c r="D30">
         <v>12</v>
       </c>
-      <c r="E29" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" s="1"/>

</xml_diff>

<commit_message>
Adicao do atributo matricula em funcionario, e implementação do acesso ao sistema
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Tarefa</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Revisão de todos os aterfatos e alterações</t>
   </si>
   <si>
-    <t xml:space="preserve">Implemetação do madança de senha </t>
-  </si>
-  <si>
     <t>Atualização na documentação</t>
   </si>
   <si>
@@ -154,13 +151,22 @@
   </si>
   <si>
     <t>1h/dia</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
+  </si>
+  <si>
+    <t>Quase completo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implemetação do mudança de senha </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,8 +196,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -208,6 +221,18 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -218,12 +243,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -232,9 +259,14 @@
     <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="16" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
+    <cellStyle name="60% - Ênfase1" xfId="3" builtinId="32"/>
+    <cellStyle name="60% - Ênfase5" xfId="4" builtinId="48"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -539,7 +571,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,12 +707,12 @@
         <v>6</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="7">
         <v>43416</v>
@@ -700,7 +732,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="7">
         <v>43414</v>
@@ -712,50 +744,50 @@
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="6" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="9">
         <v>43418</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="9">
         <v>43420</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="8">
         <v>2</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>13</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="5">
+      <c r="A10" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="11">
         <v>43421</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="11">
         <v>43423</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="10">
         <v>2</v>
       </c>
-      <c r="E10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>13</v>
+      <c r="E10" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -800,7 +832,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="5">
         <v>43429</v>
@@ -818,7 +850,7 @@
         <v>13</v>
       </c>
       <c r="G13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -843,7 +875,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" s="5">
         <v>43438</v>
@@ -863,7 +895,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="5">
         <v>43441</v>
@@ -883,7 +915,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="5">
         <v>43441</v>
@@ -903,7 +935,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="5">
         <v>43441</v>
@@ -923,7 +955,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="5">
         <v>43441</v>
@@ -943,7 +975,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="5">
         <v>43441</v>
@@ -963,7 +995,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="5">
         <v>43441</v>
@@ -983,7 +1015,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="5">
         <v>43441</v>
@@ -1003,7 +1035,7 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="5">
         <v>43441</v>
@@ -1023,7 +1055,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="5">
         <v>43450</v>
@@ -1043,7 +1075,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5">
         <v>43450</v>
@@ -1063,7 +1095,7 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="5">
         <v>43450</v>
@@ -1083,7 +1115,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="5">
         <v>43450</v>
@@ -1103,7 +1135,7 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="5">
         <v>43450</v>
@@ -1123,7 +1155,7 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="5">
         <v>43450</v>
@@ -1143,7 +1175,7 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="5">
         <v>43458</v>
@@ -1163,7 +1195,7 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="5">
         <v>43479</v>

</xml_diff>

<commit_message>
Logica do acesso ao sistema, senha sendo CNPJ ou CPF. Cadastro de clientes.
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -156,10 +156,10 @@
     <t>Em andamento</t>
   </si>
   <si>
-    <t>Quase completo</t>
-  </si>
-  <si>
     <t xml:space="preserve">Implemetação do mudança de senha </t>
+  </si>
+  <si>
+    <t>Completo</t>
   </si>
 </sst>
 </file>
@@ -204,7 +204,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -223,12 +223,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -243,14 +237,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,12 +254,9 @@
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="16" fontId="4" fillId="5" borderId="0" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="60% - Ênfase1" xfId="3" builtinId="32"/>
-    <cellStyle name="60% - Ênfase5" xfId="4" builtinId="48"/>
+  <cellStyles count="4">
+    <cellStyle name="60% - Ênfase5" xfId="3" builtinId="48"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,7 +561,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,42 +741,42 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="8" t="s">
+      <c r="A9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="9">
+      <c r="B9" s="7">
         <v>43418</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>43420</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>2</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="11">
+      <c r="B10" s="9">
         <v>43421</v>
       </c>
-      <c r="C10" s="11">
+      <c r="C10" s="9">
         <v>43423</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="8" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Reset de senha - Feito. Mudança de senha - Feito. Destalhes.
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>Tarefa</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>1h/dia</t>
-  </si>
-  <si>
-    <t>Em andamento</t>
   </si>
   <si>
     <t xml:space="preserve">Implemetação do mudança de senha </t>
@@ -197,14 +194,15 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,12 +219,6 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -237,11 +229,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -252,11 +243,10 @@
     <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="16" fontId="4" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="60% - Ênfase5" xfId="3" builtinId="48"/>
+  <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +551,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,54 +740,54 @@
       <c r="C9" s="7">
         <v>43420</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="9">
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="7">
         <v>43421</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>43423</v>
       </c>
-      <c r="D10" s="8">
+      <c r="D10" s="6">
         <v>2</v>
       </c>
-      <c r="E10" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>45</v>
+      <c r="E10" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="7">
         <v>43424</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="7">
         <v>43426</v>
       </c>
-      <c r="D11" s="4">
+      <c r="D11" s="6">
         <v>2</v>
       </c>
-      <c r="E11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>13</v>
+      <c r="E11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -816,7 +806,7 @@
       <c r="E12" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F12" s="4" t="s">
+      <c r="F12" s="8" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Logica da reserva implementada
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
   <si>
     <t>Tarefa</t>
   </si>
@@ -157,13 +157,16 @@
   </si>
   <si>
     <t>Completo</t>
+  </si>
+  <si>
+    <t>Em andamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +204,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +229,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -229,12 +245,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,10 +260,12 @@
     <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="16" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="60% - Ênfase5" xfId="3" builtinId="48"/>
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +570,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,7 +759,7 @@
       <c r="C9" s="7">
         <v>43420</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="8">
         <v>2</v>
       </c>
       <c r="E9" s="6" t="s">
@@ -791,23 +810,23 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="10">
         <v>43427</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="10">
         <v>43430</v>
       </c>
-      <c r="D12" s="4">
+      <c r="D12" s="9">
         <v>3</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>13</v>
+      <c r="E12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
logica de sair e listando as reservas - FEITO
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Correção da experição de reservas - Categoria true - Edição no documento - DML
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
   <si>
     <t>Tarefa</t>
   </si>
@@ -157,16 +157,13 @@
   </si>
   <si>
     <t>Completo</t>
-  </si>
-  <si>
-    <t>Em andamento</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -204,15 +201,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,12 +219,6 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -245,13 +229,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,11 +244,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="16" fontId="5" fillId="4" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="60% - Ênfase5" xfId="3" builtinId="48"/>
+  <cellStyles count="3">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
     <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -570,7 +551,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,7 +780,7 @@
       <c r="C11" s="7">
         <v>43426</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="9">
         <v>2</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -810,24 +791,25 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="10">
+      <c r="B12" s="7">
         <v>43427</v>
       </c>
-      <c r="C12" s="10">
+      <c r="C12" s="7">
         <v>43430</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="6">
         <v>3</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="E12" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">

</xml_diff>

<commit_message>
Atualização no documento e DER
</commit_message>
<xml_diff>
--- a/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
+++ b/DOCUMENTAÇÃO/CRONOGRAMA_PBD_2018.2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="46">
   <si>
     <t>Tarefa</t>
   </si>
@@ -55,9 +55,6 @@
   </si>
   <si>
     <t xml:space="preserve">Diagrama lógico </t>
-  </si>
-  <si>
-    <t>Não iniciado</t>
   </si>
   <si>
     <t>Implementação de todos os CRUDS</t>
@@ -187,8 +184,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -196,13 +194,13 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -212,11 +210,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -229,26 +222,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="16" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="2">
     <cellStyle name="Bom" xfId="1" builtinId="26"/>
-    <cellStyle name="Incorreto" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -550,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,236 +574,236 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="7">
+      <c r="B2" s="5">
         <v>43388</v>
       </c>
-      <c r="C2" s="7">
+      <c r="C2" s="5">
         <v>43395</v>
       </c>
-      <c r="D2" s="6">
-        <v>8</v>
-      </c>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="4">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="5">
         <v>43395</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="5">
         <v>43402</v>
       </c>
-      <c r="D3" s="6">
-        <v>8</v>
-      </c>
-      <c r="E3" s="6" t="s">
+      <c r="D3" s="4">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>43407</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="5">
         <v>43412</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="4">
         <v>5</v>
       </c>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="F4" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="7">
+      <c r="B5" s="5">
         <v>43413</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="5">
         <v>43413</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="4">
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="5">
+        <v>43414</v>
+      </c>
+      <c r="C6" s="5">
+        <v>43386</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="7">
+      <c r="F6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="5">
+        <v>43416</v>
+      </c>
+      <c r="C7" s="5">
+        <v>43417</v>
+      </c>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="5">
         <v>43414</v>
       </c>
-      <c r="C6" s="7">
-        <v>43386</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="C8" s="5">
+        <v>43414</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="5">
+        <v>43418</v>
+      </c>
+      <c r="C9" s="5">
+        <v>43420</v>
+      </c>
+      <c r="D9" s="6">
+        <v>2</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="5">
+        <v>43421</v>
+      </c>
+      <c r="C10" s="5">
+        <v>43423</v>
+      </c>
+      <c r="D10" s="4">
+        <v>2</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5">
+        <v>43424</v>
+      </c>
+      <c r="C11" s="5">
+        <v>43426</v>
+      </c>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" s="5">
+        <v>43427</v>
+      </c>
+      <c r="C12" s="5">
+        <v>43430</v>
+      </c>
+      <c r="D12" s="4">
         <v>3</v>
       </c>
-      <c r="E6" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B7" s="7">
-        <v>43416</v>
-      </c>
-      <c r="C7" s="7">
-        <v>43417</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="7">
-        <v>43414</v>
-      </c>
-      <c r="C8" s="7">
-        <v>43414</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="7">
-        <v>43418</v>
-      </c>
-      <c r="C9" s="7">
-        <v>43420</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B10" s="7">
-        <v>43421</v>
-      </c>
-      <c r="C10" s="7">
-        <v>43423</v>
-      </c>
-      <c r="D10" s="6">
-        <v>2</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11" s="7">
-        <v>43424</v>
-      </c>
-      <c r="C11" s="7">
-        <v>43426</v>
-      </c>
-      <c r="D11" s="9">
-        <v>2</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12" s="7">
-        <v>43427</v>
-      </c>
-      <c r="C12" s="7">
-        <v>43430</v>
-      </c>
-      <c r="D12" s="6">
-        <v>3</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="6" t="s">
+      <c r="E12" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="G12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B13" s="5">
         <v>43429</v>
@@ -825,18 +815,18 @@
         <v>1</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="G13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="5">
         <v>43431</v>
@@ -851,12 +841,12 @@
         <v>11</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="5">
         <v>43438</v>
@@ -871,12 +861,12 @@
         <v>11</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B16" s="5">
         <v>43441</v>
@@ -888,15 +878,15 @@
         <v>3</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" s="5">
         <v>43441</v>
@@ -908,15 +898,15 @@
         <v>8</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="5">
         <v>43441</v>
@@ -928,15 +918,15 @@
         <v>8</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="5">
         <v>43441</v>
@@ -948,15 +938,15 @@
         <v>8</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B20" s="5">
         <v>43441</v>
@@ -968,15 +958,15 @@
         <v>8</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B21" s="5">
         <v>43441</v>
@@ -988,15 +978,15 @@
         <v>8</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22" s="5">
         <v>43441</v>
@@ -1008,15 +998,15 @@
         <v>8</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B23" s="5">
         <v>43441</v>
@@ -1028,15 +1018,15 @@
         <v>8</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B24" s="5">
         <v>43450</v>
@@ -1048,15 +1038,15 @@
         <v>8</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5">
         <v>43450</v>
@@ -1068,15 +1058,16 @@
         <v>8</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="5">
         <v>43450</v>
@@ -1088,15 +1079,15 @@
         <v>8</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B27" s="5">
         <v>43450</v>
@@ -1108,15 +1099,15 @@
         <v>8</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B28" s="5">
         <v>43450</v>
@@ -1128,15 +1119,15 @@
         <v>8</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B29" s="5">
         <v>43450</v>
@@ -1148,15 +1139,15 @@
         <v>8</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B30" s="5">
         <v>43458</v>
@@ -1168,15 +1159,15 @@
         <v>23</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B31" s="5">
         <v>43479</v>
@@ -1188,13 +1179,13 @@
         <v>12</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F31" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>

</xml_diff>